<commit_message>
- CSS - ToDo edit
</commit_message>
<xml_diff>
--- a/doc/ToDo.xlsx
+++ b/doc/ToDo.xlsx
@@ -7,19 +7,17 @@
     <workbookView xWindow="600" yWindow="30" windowWidth="19395" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="ToDo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ToDo!$A$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Fragen</t>
   </si>
@@ -73,6 +71,42 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Erledigt?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Wer?</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>F12 im Chrome</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Bei Neu: Überkategorie kann nicht ausgewählt werden</t>
+  </si>
+  <si>
+    <t>Alle Warnings und Fehler nicht auf der Seite anzeigen</t>
+  </si>
+  <si>
+    <t>Datenbank online bringen</t>
+  </si>
+  <si>
+    <t>Footer entfernen</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt; kleinere Schriftgröße klappt nicht</t>
   </si>
 </sst>
 </file>
@@ -114,9 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,133 +448,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" hidden="1">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" hidden="1">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B2"/>
+  <autoFilter ref="A1:D15">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- DB dump - Update ToDo
</commit_message>
<xml_diff>
--- a/doc/ToDo.xlsx
+++ b/doc/ToDo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Fragen</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Auswertungen/Diagramme erstellen</t>
+  </si>
+  <si>
+    <t>Zum Blättern in Seiten unterteilen, 20 Fragen pro Seite</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -674,6 +677,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F16">
     <filterColumn colId="3">

</xml_diff>

<commit_message>
- Benutzer bearbeiten (fertig) - Statistiken (fertig)
</commit_message>
<xml_diff>
--- a/doc/ToDo.xlsx
+++ b/doc/ToDo.xlsx
@@ -10,14 +10,14 @@
     <sheet name="ToDo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ToDo!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ToDo!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Fragen</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Alle Warnings und Fehler nicht auf der Seite anzeigen</t>
   </si>
   <si>
-    <t>Datenbank online bringen</t>
-  </si>
-  <si>
     <t>Footer entfernen</t>
   </si>
   <si>
@@ -113,6 +110,12 @@
   </si>
   <si>
     <t>Zum Blättern in Seiten unterteilen, 20 Fragen pro Seite</t>
+  </si>
+  <si>
+    <t>Datenbank und Rest online bringen (multiplechoice.szüsz.de)</t>
+  </si>
+  <si>
+    <t>Suchen nach zu 0</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -575,19 +578,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -597,7 +602,9 @@
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:6" hidden="1">
       <c r="A11" t="s">
@@ -628,7 +635,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -638,14 +645,19 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
@@ -657,7 +669,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -671,7 +683,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>20</v>
@@ -682,14 +694,14 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F16">
+  <autoFilter ref="A1:F17">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
- ToDo aktualisiert - Navigation überarbeitet
</commit_message>
<xml_diff>
--- a/doc/ToDo.xlsx
+++ b/doc/ToDo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Fragen</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>x?</t>
+  </si>
+  <si>
+    <t>Pulldown?</t>
   </si>
 </sst>
 </file>
@@ -168,7 +174,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -176,9 +182,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,7 +222,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -286,7 +292,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -464,10 +470,10 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.375" bestFit="1" customWidth="1"/>
@@ -504,7 +510,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6">
@@ -518,7 +526,10 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1">
@@ -535,7 +546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -549,7 +560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -570,7 +581,9 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:6" hidden="1">
@@ -632,7 +645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -689,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -699,8 +712,11 @@
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -710,11 +726,14 @@
       <c r="C17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F17">
     <filterColumn colId="3">
-      <filters blank="1"/>
+      <filters blank="1">
+        <filter val="x?"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- keine Fehler werden mehr angezeigt (conf.php) - Fragen Bearbeitet überarbeitet
</commit_message>
<xml_diff>
--- a/doc/ToDo.xlsx
+++ b/doc/ToDo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Fragen</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>x?</t>
-  </si>
-  <si>
-    <t>Pulldown?</t>
   </si>
 </sst>
 </file>
@@ -470,7 +464,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -515,7 +509,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -526,10 +520,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1">
@@ -731,9 +722,7 @@
   </sheetData>
   <autoFilter ref="A1:F17">
     <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="x?"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>